<commit_message>
19,12,2024 dodane dwa zestawy danych, aor1_rna do poprawy
</commit_message>
<xml_diff>
--- a/datasets/data database.xlsx
+++ b/datasets/data database.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B579C0-5DD8-42AC-9B01-3141A3B109A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFAAF0A-C05F-4170-BDB1-4C2D9118393D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="240" windowWidth="14370" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>data</t>
   </si>
@@ -61,6 +72,24 @@
   </si>
   <si>
     <t>mutant strain S. coelicolor M145 ∆abrB relative to wild type in NMMP at 36 hours</t>
+  </si>
+  <si>
+    <t>abrc3</t>
+  </si>
+  <si>
+    <t>abrC3 mutant relative to the parent strain M145</t>
+  </si>
+  <si>
+    <t>absaA2_scoe</t>
+  </si>
+  <si>
+    <t>troche nie wiem co z tym zrobić</t>
+  </si>
+  <si>
+    <t>aor1_rna</t>
+  </si>
+  <si>
+    <t>Genes whose transcript levels changed at least 3-fold (FC) in S. coelicolor ∆aor1 compared with those of M145</t>
   </si>
 </sst>
 </file>
@@ -644,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,27 +769,43 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="17"/>
+      <c r="D9" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="17"/>
+      <c r="B10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
o matulu, pierwszy commit nowego roku, bo zapominam to robić, 16.01.2025
</commit_message>
<xml_diff>
--- a/datasets/data database.xlsx
+++ b/datasets/data database.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFAAF0A-C05F-4170-BDB1-4C2D9118393D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFC1634-E27D-42D6-868D-90C8865A3598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="240" windowWidth="14370" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="0" windowWidth="14370" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="database" sheetId="1" r:id="rId1"/>
+    <sheet name="zmienne_sven" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="129">
   <si>
     <t>data</t>
   </si>
@@ -90,19 +91,444 @@
   </si>
   <si>
     <t>Genes whose transcript levels changed at least 3-fold (FC) in S. coelicolor ∆aor1 compared with those of M145</t>
+  </si>
+  <si>
+    <t>argR_2018</t>
+  </si>
+  <si>
+    <t>bldD_scoe</t>
+  </si>
+  <si>
+    <t>bobek_streptomyces germination</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>omówić na spotkaniu</t>
+  </si>
+  <si>
+    <t>draRK_scoe</t>
+  </si>
+  <si>
+    <t>genbankfiles</t>
+  </si>
+  <si>
+    <t>omówić</t>
+  </si>
+  <si>
+    <t>glmr_sven</t>
+  </si>
+  <si>
+    <t>hupBlsr_rnaseq</t>
+  </si>
+  <si>
+    <t>hupS_rnaseq_Strzalka</t>
+  </si>
+  <si>
+    <t>monika_tnseq</t>
+  </si>
+  <si>
+    <t>NapM</t>
+  </si>
+  <si>
+    <t>ohkA_scoe</t>
+  </si>
+  <si>
+    <t>osdR_2016</t>
+  </si>
+  <si>
+    <t>ppgpp_scoe</t>
+  </si>
+  <si>
+    <t>rnasell_scoe</t>
+  </si>
+  <si>
+    <t>scoe_cogs</t>
+  </si>
+  <si>
+    <t>scoe_pfam</t>
+  </si>
+  <si>
+    <t>sigB</t>
+  </si>
+  <si>
+    <t>sigR</t>
+  </si>
+  <si>
+    <t>soxR</t>
+  </si>
+  <si>
+    <t>strzalka_hupAS</t>
+  </si>
+  <si>
+    <t>sven_kim_woori</t>
+  </si>
+  <si>
+    <t>wbIA_scoe</t>
+  </si>
+  <si>
+    <t>whiA_sven</t>
+  </si>
+  <si>
+    <t>whiAH_scoe</t>
+  </si>
+  <si>
+    <t>yague_2013_scoe_diff</t>
+  </si>
+  <si>
+    <t>yeong_2016</t>
+  </si>
+  <si>
+    <t>DNA microarray analysis identifies 359 genes that are significantly and &gt;2-fold differently expressed as a result of bldD deletion</t>
+  </si>
+  <si>
+    <t>Microarray</t>
+  </si>
+  <si>
+    <t>nie mam pojęcia co to za wyniki i jak je interpretować</t>
+  </si>
+  <si>
+    <t>uploaded_file</t>
+  </si>
+  <si>
+    <t>output.fileUploaded</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>select_gene</t>
+  </si>
+  <si>
+    <t>rna_select_1</t>
+  </si>
+  <si>
+    <t>contrast_1</t>
+  </si>
+  <si>
+    <t>rna_select_2</t>
+  </si>
+  <si>
+    <t>contrast_2</t>
+  </si>
+  <si>
+    <t>rna_select_3</t>
+  </si>
+  <si>
+    <t>contrast_3</t>
+  </si>
+  <si>
+    <t>wybor</t>
+  </si>
+  <si>
+    <t>btn_left</t>
+  </si>
+  <si>
+    <t>btn_right</t>
+  </si>
+  <si>
+    <t>btn_in</t>
+  </si>
+  <si>
+    <t>btn_out</t>
+  </si>
+  <si>
+    <t>lower_value</t>
+  </si>
+  <si>
+    <t>higher_value</t>
+  </si>
+  <si>
+    <t>higher_logFC</t>
+  </si>
+  <si>
+    <t>lower_logFC</t>
+  </si>
+  <si>
+    <t>my_switch</t>
+  </si>
+  <si>
+    <t>switch_status</t>
+  </si>
+  <si>
+    <t>all_plots</t>
+  </si>
+  <si>
+    <t>rna_table</t>
+  </si>
+  <si>
+    <t>chip_table</t>
+  </si>
+  <si>
+    <t>gene_protein_data</t>
+  </si>
+  <si>
+    <t>uploaded_file_sven</t>
+  </si>
+  <si>
+    <t>output.fileUploaded_sven</t>
+  </si>
+  <si>
+    <t>file_name_sven</t>
+  </si>
+  <si>
+    <t>options_sven</t>
+  </si>
+  <si>
+    <t>select_gene_sven</t>
+  </si>
+  <si>
+    <t>rna_select_1_sven</t>
+  </si>
+  <si>
+    <t>contrast_1_sven</t>
+  </si>
+  <si>
+    <t>rna_select_2_sven</t>
+  </si>
+  <si>
+    <t>contrast_2_sven</t>
+  </si>
+  <si>
+    <t>rna_select_3_sven</t>
+  </si>
+  <si>
+    <t>contrast_3_sven</t>
+  </si>
+  <si>
+    <t>wybor_sven</t>
+  </si>
+  <si>
+    <t>btn_left_sven</t>
+  </si>
+  <si>
+    <t>btn_right_sven</t>
+  </si>
+  <si>
+    <t>btn_in_sven</t>
+  </si>
+  <si>
+    <t>btn_out_sven</t>
+  </si>
+  <si>
+    <t>lower_value_sven</t>
+  </si>
+  <si>
+    <t>higher_value_sven</t>
+  </si>
+  <si>
+    <t>higher_logFC_sven</t>
+  </si>
+  <si>
+    <t>lower_logFC_sven</t>
+  </si>
+  <si>
+    <t>my_switch_sven</t>
+  </si>
+  <si>
+    <t>switch_status_sven</t>
+  </si>
+  <si>
+    <t>all_plots_sven</t>
+  </si>
+  <si>
+    <t>rna_table_sven</t>
+  </si>
+  <si>
+    <t>chip_table_sven</t>
+  </si>
+  <si>
+    <t>gene_protein_data_sven</t>
+  </si>
+  <si>
+    <t>differentiation of the ∆draR-K mutant relative to the parental strain M145</t>
+  </si>
+  <si>
+    <t>ECF42s_sven</t>
+  </si>
+  <si>
+    <t>zrobione</t>
+  </si>
+  <si>
+    <t>dodane do app</t>
+  </si>
+  <si>
+    <t>tak</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table S5. Genes differentially transcribed between S. coelicolor M145 and S. coelicolor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>argR</t>
+    </r>
+  </si>
+  <si>
+    <t>nie</t>
+  </si>
+  <si>
+    <t>noinfo</t>
+  </si>
+  <si>
+    <t>do omówienia MSMEG</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Some key functional genes whose transcription was down- or up-regulated over twofold due to the deletion of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ohkA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> gene.</t>
+    </r>
+  </si>
+  <si>
+    <t>rna-seq</t>
+  </si>
+  <si>
+    <t>Global transcription profiling of the osdR null mutant by DNA microarray analysis. P</t>
+  </si>
+  <si>
+    <t>microarray</t>
+  </si>
+  <si>
+    <t>tylko p_value dostępne z awartości</t>
+  </si>
+  <si>
+    <t>nie nie</t>
+  </si>
+  <si>
+    <t>we have examined the transcriptomes of S. coelicolor
+M145 and an RNase III (rnc)-null mutant of that strain. RNA preparations with reduced levels of structural RNAs were prepared
+by subtractive hybridization prior to RNA-Seq analysis. We initially identified 7,800 transcripts of known and putative proteincoding genes in M145 and the null mutant, JSE1880, alon</t>
+  </si>
+  <si>
+    <t>brak danych do prezentacji</t>
+  </si>
+  <si>
+    <t>sigR deletion</t>
+  </si>
+  <si>
+    <t>we conducted a whole genome transcriptome comparison of wild type S. coelicolor and a soxR-deficient mutant in stationary phase using RNA-Seq.</t>
+  </si>
+  <si>
+    <t>jest jakimś binarnopodobnym i się nie otwiera</t>
+  </si>
+  <si>
+    <t>nie rozimiem zapisu genów, możliwe że jakieś analogi</t>
+  </si>
+  <si>
+    <t>brak sensownych wyników do prezentacji</t>
+  </si>
+  <si>
+    <t>nie rozumiem co się dzieje wtych danych, mało podpisów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genes that are differentially expressed when compring whiA or whiH mutant to wildtype parent, or comparing the developing wildtype strain at 36 h or 48 h to the expression pattern at 18 h. </t>
+  </si>
+  <si>
+    <t>data_bldC</t>
+  </si>
+  <si>
+    <t>wywalone troche NA bo nie było genów w liście</t>
+  </si>
+  <si>
+    <t>analysis of the role of GlnR by nitrogen starvation (deletion of glnr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="4">
@@ -125,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -253,21 +679,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -356,33 +767,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -391,11 +799,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Normal 8 11" xfId="1" xr:uid="{59EAA117-2FEB-4110-8EC0-2CC4C4AF92C2}"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -671,610 +1188,1290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="9"/>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="11"/>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="11"/>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="22"/>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
+      <c r="F8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="22"/>
+      <c r="F9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="22"/>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="29"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="29"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="29"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="12"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="10"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="10"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="10"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="10"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="10"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="12"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="12"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="12"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="12"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="11"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="12"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="12"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="12"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="11"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="12"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="11"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="12"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="12"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="12"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="11"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="12"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="11"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="11"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="12"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="10"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="4"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="13"/>
       <c r="D61" s="17"/>
-      <c r="E61" s="12"/>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3">
+      <c r="E61" s="14"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H24:H25 F3:G61">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="nie">
+      <formula>NOT(ISERROR(SEARCH("nie",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="tak">
+      <formula>NOT(ISERROR(SEARCH("tak",F3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="nie">
+      <formula>NOT(ISERROR(SEARCH("nie",H27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="tak">
+      <formula>NOT(ISERROR(SEARCH("tak",H27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="nie">
+      <formula>NOT(ISERROR(SEARCH("nie",H31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="tak">
+      <formula>NOT(ISERROR(SEARCH("tak",H31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="nie">
+      <formula>NOT(ISERROR(SEARCH("nie",H32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="tak">
+      <formula>NOT(ISERROR(SEARCH("tak",H32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A829A2A-901F-49B9-9542-2534F2B9AFF1}">
+  <dimension ref="C2:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="15"/>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
29.01.2025 pt2 dodany nowy zestaw danych,
</commit_message>
<xml_diff>
--- a/datasets/data database.xlsx
+++ b/datasets/data database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94361CF0-A98F-4324-901B-48FCFB2C4C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91A90C2-0238-44EB-82CF-4FF2AAF99AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="0" windowWidth="14370" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="133">
   <si>
     <t>data</t>
   </si>
@@ -477,6 +477,14 @@
   </si>
   <si>
     <t>Supplementary Data 5. Compilation of genes differentially expressed at different growth phases. The expression values for replicate data were merged as a normalized value by DESeq. Among the four time points, only genes have normalized mRNA expression level greater than cutoff value (= 32.8; see Methods) for at least one time point were considered. Comparing every two time points, genes having mRNA fold changes over 2 and p-value smaller than 0.05 (calculated by DESeq) were listed. M, mid-exponential; T, transition; L, late exponential and S, stationary phase. In Row 2, M vs. T means T/M.</t>
+  </si>
+  <si>
+    <t>sven_NRRL_metab_RNAseq</t>
+  </si>
+  <si>
+    <t>Targeted Metabolomics and High-Throughput RNA SequencingBased Transcriptomics Reveal Massive Changes in the
+Streptomyces venezuelae NRRL B-65442 Metabolism Caused by
+Ethanol Shock</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1184,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,10 +2032,22 @@
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="16"/>
+      <c r="B40" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>132</v>
+      </c>
       <c r="E40" s="11"/>
+      <c r="F40" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">

</xml_diff>

<commit_message>
23.02.2025 pozmieniane ogólnie UI aplikacji i jej nazwa; download ploty działają wszystkie; dane RNAseq i CHipseq mają sensowniejsze nazwwy; dodano opcje wczytania danych chipseq, ale nie w formacie bad tylko tekstowym oddzielonym tabulatorami, bo coś nie styka z wczytywaniem BEDów; intime-comp - do omówienia; poprawiony wykres chip-seq; przy zmianie gatunku, zmieniają się dostępne dane; Help&info, nie ruszone; dane poprawione według uwag w excelu;
</commit_message>
<xml_diff>
--- a/datasets/data database.xlsx
+++ b/datasets/data database.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A63EC7AC-30F4-485E-BF33-E175F1ACD2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532CF497-2DBE-4FE4-981D-AC9EB057AECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="0" windowWidth="14370" windowHeight="15510" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="1005" windowWidth="12420" windowHeight="13890" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
     <sheet name="zmienne_sven" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="180">
   <si>
     <t>data</t>
   </si>
@@ -327,9 +340,6 @@
 by subtractive hybridization prior to RNA-Seq analysis. We initially identified 7,800 transcripts of known and putative proteincoding genes in M145 and the null mutant, JSE1880, alon</t>
   </si>
   <si>
-    <t>nie mogę znaleźć w aplikacji</t>
-  </si>
-  <si>
     <t>scoe_cogs</t>
   </si>
   <si>
@@ -579,6 +589,54 @@
   </si>
   <si>
     <t>poprawione</t>
+  </si>
+  <si>
+    <t>połączone, nazwa zmienona na Aor1_Antoraz_2017</t>
+  </si>
+  <si>
+    <t>dane poprawione nazwa zmieniopna na argr_botas_2018</t>
+  </si>
+  <si>
+    <t>policzonelogfc, nazwa zmieniona BldD_denHengst_2010</t>
+  </si>
+  <si>
+    <t>poprawione z tymi czasami, zmieniona nazwa na BldC_Bush_2018_sven</t>
+  </si>
+  <si>
+    <t>zmieniona nazwa Drar-K_Yu_2014</t>
+  </si>
+  <si>
+    <t>poprawione, nazwa ECF42_Liu_2018_sven</t>
+  </si>
+  <si>
+    <t>poprawiony ten czas, ale nie wiem jak odróżnić które geny z tym azotem. Nazwa zmieniona na GlnR_Pullan_2011</t>
+  </si>
+  <si>
+    <t>usunięte</t>
+  </si>
+  <si>
+    <t>zlogarytmowane, bo nie było logarytmowane, nazwa zmieniona na OhkA_Lu_2011</t>
+  </si>
+  <si>
+    <t>zlogarytmowane, nazwa OsdR_Urem_2016</t>
+  </si>
+  <si>
+    <t>nazwa zmieniona sigR_Kallifidas_2010</t>
+  </si>
+  <si>
+    <t>nazwa zmieniona soxR_Naseer_2014</t>
+  </si>
+  <si>
+    <t>nazwa zmieniopna whiAH_Salerno_2013</t>
+  </si>
+  <si>
+    <t>poprawuobe rozróżnienie na solid/liquid, nazwa zmienionba na SolidLiquidDiff_Yague_2013</t>
+  </si>
+  <si>
+    <t>poprawione, nazwa growth_phases_yeong_2016</t>
+  </si>
+  <si>
+    <t>zmienbniona nazwa</t>
   </si>
 </sst>
 </file>
@@ -904,7 +962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -964,6 +1022,7 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 8 11" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1323,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1422,7 @@
         <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1389,7 +1448,7 @@
         <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1415,7 +1474,7 @@
         <v>13</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1441,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1540,7 +1599,7 @@
       </c>
       <c r="J8" s="11"/>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
@@ -1601,9 +1660,11 @@
       </c>
       <c r="J10" s="11"/>
       <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>164</v>
+      </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
@@ -1635,9 +1696,11 @@
       </c>
       <c r="J11" s="23"/>
       <c r="K11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="L11" s="35" t="s">
+        <v>165</v>
+      </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
     </row>
@@ -1669,9 +1732,11 @@
       </c>
       <c r="J12" s="11"/>
       <c r="K12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>166</v>
+      </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
     </row>
@@ -1731,9 +1796,11 @@
       </c>
       <c r="J14" s="11"/>
       <c r="K14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>167</v>
+      </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11"/>
     </row>
@@ -1791,13 +1858,15 @@
       </c>
       <c r="J16" s="11"/>
       <c r="K16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>168</v>
+      </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
@@ -1822,10 +1891,13 @@
         <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
@@ -1843,7 +1915,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
@@ -1868,10 +1940,13 @@
         <v>59</v>
       </c>
       <c r="K19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>18</v>
       </c>
@@ -1890,7 +1965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
@@ -1912,10 +1987,13 @@
         <v>63</v>
       </c>
       <c r="K21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>20</v>
       </c>
@@ -1934,7 +2012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>21</v>
       </c>
@@ -1953,7 +2031,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>22</v>
       </c>
@@ -1980,10 +2058,13 @@
         <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>23</v>
       </c>
@@ -2010,10 +2091,13 @@
         <v>74</v>
       </c>
       <c r="K25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>24</v>
       </c>
@@ -2035,7 +2119,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>25</v>
       </c>
@@ -2050,25 +2134,23 @@
       </c>
       <c r="E27" s="16"/>
       <c r="F27" s="11" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>26</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="11" t="s">
@@ -2078,16 +2160,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>27</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E29" s="16"/>
       <c r="F29" s="11" t="s">
@@ -2097,16 +2179,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>28</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="11" t="s">
@@ -2116,18 +2198,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>29</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="11" t="s">
@@ -2137,19 +2219,22 @@
         <v>9</v>
       </c>
       <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>30</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="11" t="s">
@@ -2160,22 +2245,25 @@
       </c>
       <c r="H32" s="17"/>
       <c r="I32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>31</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="11" t="s">
@@ -2185,16 +2273,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>32</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="11" t="s">
@@ -2204,19 +2292,19 @@
         <v>28</v>
       </c>
       <c r="I34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>33</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="11" t="s">
@@ -2226,16 +2314,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>34</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="11" t="s">
@@ -2245,24 +2333,24 @@
         <v>28</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K36" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>35</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E37" s="16"/>
       <c r="F37" t="s">
@@ -2278,21 +2366,24 @@
         <v>51</v>
       </c>
       <c r="K37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>36</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>71</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="11" t="s">
@@ -2305,22 +2396,25 @@
         <v>35</v>
       </c>
       <c r="I38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K38" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>37</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="11" t="s">
@@ -2333,24 +2427,27 @@
         <v>35</v>
       </c>
       <c r="I39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>38</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="11" t="s">
@@ -2359,8 +2456,11 @@
       <c r="G40" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>39</v>
       </c>
@@ -2369,7 +2469,7 @@
       <c r="D41" s="15"/>
       <c r="E41" s="16"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>40</v>
       </c>
@@ -2378,7 +2478,7 @@
       <c r="D42" s="15"/>
       <c r="E42" s="16"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>41</v>
       </c>
@@ -2387,10 +2487,10 @@
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
       <c r="I43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>42</v>
       </c>
@@ -2399,7 +2499,7 @@
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>43</v>
       </c>
@@ -2408,7 +2508,7 @@
       <c r="D45" s="15"/>
       <c r="E45" s="16"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>44</v>
       </c>
@@ -2417,7 +2517,7 @@
       <c r="D46" s="15"/>
       <c r="E46" s="16"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>45</v>
       </c>
@@ -2426,7 +2526,7 @@
       <c r="D47" s="15"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>46</v>
       </c>
@@ -2585,7 +2685,7 @@
       <formula>NOT(ISERROR(SEARCH("tak",H31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="K1:K1048576 L24:L25 L32 L37:L40">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="tak">
       <formula>NOT(ISERROR(SEARCH("tak",K1)))</formula>
     </cfRule>
@@ -2613,210 +2713,210 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
         <v>114</v>
-      </c>
-      <c r="D3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
         <v>116</v>
-      </c>
-      <c r="D4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
         <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
         <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
         <v>122</v>
-      </c>
-      <c r="D7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
         <v>124</v>
-      </c>
-      <c r="D8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
         <v>126</v>
-      </c>
-      <c r="D9" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" t="s">
         <v>128</v>
-      </c>
-      <c r="D10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
         <v>132</v>
-      </c>
-      <c r="D12" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" t="s">
         <v>134</v>
-      </c>
-      <c r="D13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" t="s">
         <v>136</v>
-      </c>
-      <c r="D14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" t="s">
         <v>138</v>
-      </c>
-      <c r="D15" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" t="s">
         <v>140</v>
-      </c>
-      <c r="D16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" t="s">
         <v>142</v>
-      </c>
-      <c r="D17" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
         <v>144</v>
-      </c>
-      <c r="D18" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" t="s">
         <v>146</v>
-      </c>
-      <c r="D19" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
         <v>148</v>
-      </c>
-      <c r="D20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
         <v>150</v>
-      </c>
-      <c r="D21" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" t="s">
         <v>152</v>
-      </c>
-      <c r="D22" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
         <v>154</v>
-      </c>
-      <c r="D23" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" t="s">
         <v>156</v>
-      </c>
-      <c r="D24" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" t="s">
         <v>158</v>
-      </c>
-      <c r="D25" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" t="s">
         <v>160</v>
-      </c>
-      <c r="D26" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="s">
         <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>